<commit_message>
updated template for enrollment certificate
</commit_message>
<xml_diff>
--- a/static/templates/enrollment_certificate-template.xlsx
+++ b/static/templates/enrollment_certificate-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Republic of the Philippines</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">Bicol University</t>
   </si>
   <si>
-    <t xml:space="preserve">Tel. No.</t>
-  </si>
-  <si>
     <t xml:space="preserve">ISO 9001:2008</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">           Issued this for reference purposes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrar</t>
   </si>
   <si>
     <t xml:space="preserve">BU-F-UREG-11</t>
@@ -71,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -101,9 +95,25 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b val="true"/>
+      <sz val="20"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -149,7 +159,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -158,7 +168,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -170,8 +180,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -191,15 +217,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>121320</xdr:colOff>
+      <xdr:colOff>121680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>880920</xdr:colOff>
+      <xdr:colOff>880200</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -212,8 +238,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1140480" y="600480"/>
-          <a:ext cx="759600" cy="842040"/>
+          <a:off x="1144440" y="601200"/>
+          <a:ext cx="758520" cy="840960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -233,13 +259,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:I42"/>
+  <dimension ref="B4:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
@@ -270,33 +296,30 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -307,71 +330,99 @@
       <c r="I15" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F31" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F33" s="8"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F34" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="D6:G6"/>
@@ -379,8 +430,9 @@
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="B20:G22"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>